<commit_message>
cambie las instancias del 2
</commit_message>
<xml_diff>
--- a/informe/imgs/ejemplosEj2.xlsx
+++ b/informe/imgs/ejemplosEj2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="16740" tabRatio="141"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25540" windowHeight="14080" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>1)</t>
-  </si>
-  <si>
-    <t>2)</t>
-  </si>
-  <si>
-    <t>3)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Curso nº1</t>
   </si>
@@ -46,17 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -69,7 +52,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,12 +79,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -119,13 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -138,7 +112,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -542,255 +515,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M31"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="77" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" customHeight="1"/>
-    <row r="2" spans="2:13" ht="15" customHeight="1">
-      <c r="C2" s="1">
+    <row r="1" spans="1:14" ht="15" customHeight="1">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="J2" s="1">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="K2" s="1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="L2" s="1">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="M2" s="1">
+      <c r="K1" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
+    <row r="2" spans="1:14" ht="15" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" customHeight="1">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="2:13" ht="16" customHeight="1">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="2:13" ht="15" customHeight="1">
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="2:13" ht="56.75" customHeight="1"/>
-    <row r="8" spans="2:13" ht="15" customHeight="1">
-      <c r="C8" s="1">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" customHeight="1">
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1"/>
+    <row r="7" spans="1:14" ht="56.75" customHeight="1">
+      <c r="A7" s="1">
         <v>0</v>
       </c>
-      <c r="D8" s="1">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="1">
+      <c r="E7" s="1">
         <v>4</v>
       </c>
-      <c r="H8" s="1">
+      <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="G7" s="1">
         <v>6</v>
       </c>
-      <c r="J8" s="1">
+      <c r="H7" s="1">
         <v>7</v>
       </c>
-      <c r="K8" s="1">
+      <c r="I7" s="1">
         <v>8</v>
       </c>
-      <c r="L8" s="1">
+      <c r="J7" s="1">
         <v>9</v>
       </c>
-      <c r="M8" s="1">
+      <c r="K7" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15" customHeight="1">
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="8" spans="1:14" ht="15" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1">
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:13" ht="15" customHeight="1">
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+    <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:13" ht="15" customHeight="1">
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="2:13" ht="15" customHeight="1">
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="2:13" ht="56.75" customHeight="1"/>
-    <row r="14" spans="2:13" ht="15" customHeight="1"/>
-    <row r="15" spans="2:13" ht="15" customHeight="1">
-      <c r="C15" s="1">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1"/>
+    <row r="13" spans="1:14" ht="56.75" customHeight="1"/>
+    <row r="14" spans="1:14" ht="20" customHeight="1"/>
+    <row r="15" spans="1:14" ht="15" customHeight="1">
+      <c r="B15" s="6"/>
+      <c r="C15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1">
+      <c r="C16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+    </row>
+    <row r="17" spans="2:14" ht="15" customHeight="1">
+      <c r="B17" s="7"/>
+      <c r="C17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="2:14" ht="15" customHeight="1">
+      <c r="C18" s="9"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="2:14" ht="15" customHeight="1">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="1">
+    </row>
+    <row r="20" spans="2:14" ht="15" customHeight="1"/>
+    <row r="21" spans="2:14" ht="15" customHeight="1">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
-      <c r="H15" s="1">
-        <v>5</v>
-      </c>
-      <c r="I15" s="1">
-        <v>6</v>
-      </c>
-      <c r="J15" s="1">
-        <v>7</v>
-      </c>
-      <c r="K15" s="1">
-        <v>8</v>
-      </c>
-      <c r="L15" s="1">
-        <v>9</v>
-      </c>
-      <c r="M15" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="15" customHeight="1">
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="3:11" ht="15" customHeight="1">
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="3:11" ht="15" customHeight="1">
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="3:11" ht="15" customHeight="1"/>
-    <row r="20" spans="3:11" ht="15" customHeight="1"/>
-    <row r="21" spans="3:11" ht="15" customHeight="1"/>
-    <row r="22" spans="3:11" ht="15" customHeight="1"/>
-    <row r="23" spans="3:11" ht="15" customHeight="1"/>
-    <row r="24" spans="3:11" ht="15" customHeight="1"/>
-    <row r="25" spans="3:11" ht="15" customHeight="1">
-      <c r="C25" s="7"/>
-      <c r="D25" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" ht="15" customHeight="1">
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="3:11" ht="15" customHeight="1">
-      <c r="C27" s="8"/>
-      <c r="D27" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" ht="15" customHeight="1">
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="3:11" ht="15" customHeight="1">
-      <c r="C29" s="9"/>
-      <c r="D29" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="3:11">
-      <c r="C31" s="12"/>
-      <c r="D31" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    </row>
+    <row r="22" spans="2:14" ht="15" customHeight="1"/>
+    <row r="23" spans="2:14" ht="15" customHeight="1"/>
+    <row r="24" spans="2:14" ht="15" customHeight="1"/>
+    <row r="25" spans="2:14" ht="15" customHeight="1"/>
+    <row r="26" spans="2:14" ht="15" customHeight="1"/>
+    <row r="27" spans="2:14" ht="15" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="3.9583333333333297E-2" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="66" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="12" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>